<commit_message>
Add basic levels and structure.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -2,18 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28919"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{510BEAA0-F501-45F4-A324-A2158B3843D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6DA363-49D5-4116-A14A-B2B6BA7E8E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2805" yWindow="3120" windowWidth="26925" windowHeight="13725" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Workings" sheetId="1" r:id="rId1"/>
+    <sheet name="Information" sheetId="2" r:id="rId2"/>
+    <sheet name="L1_ChooseAStarter" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +37,40 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>XLOOKUP</t>
+  </si>
+  <si>
+    <t>INDEX</t>
+  </si>
+  <si>
+    <t>VLOOKUP</t>
+  </si>
+  <si>
+    <t>Selection:</t>
+  </si>
+  <si>
+    <t>Please select your selection function, enter its name in the 'finished' box, and then recalculate the sheet.</t>
+  </si>
+  <si>
+    <t>Level Deadline</t>
+  </si>
+  <si>
+    <t>Active Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time Remaining </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="20"/>
@@ -46,15 +80,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -62,12 +102,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +466,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBED99E-4F78-4FBF-8396-4E9D77C4649A}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <sheetData/>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FEC854-5F2C-4439-9B10-91385C4E6F6F}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="B2:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="20.78515625" customWidth="1"/>
+    <col min="3" max="3" width="21.0703125" customWidth="1"/>
+    <col min="4" max="4" width="23.640625" customWidth="1"/>
+    <col min="5" max="5" width="16.0703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2">
+        <f ca="1">D3-NOW()</f>
+        <v>9.0181597217451781E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>45809.662609606479</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="rj0B5JYqci1h/lqRC1ahyCTMcZHzmNQg98Pej68Ur7uJQe0diBpa8fqaK2MSFLaC7DPMzieNdJoZUM0Fqg0aqQ==" saltValue="R7DkZ+5Vy9VG8zZTowy73w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC1F9E8-8D01-42FA-A050-785391142542}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="B2:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="IV8TLPBvCGQR47d9G6goayeZFTssMGfqzsIyX8zTfRwz1J+yJ7UgvO7C74FtCUKOH9KwUQzqYQ/Ik1OxyhN8mw==" saltValue="+YR3yY6BtJL6ni7ZkNRWVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Set up the skeleton for the first rival battle.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6DA363-49D5-4116-A14A-B2B6BA7E8E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6219DCB3-BD24-4EAC-81E1-80C34EB6CA05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="38700" windowHeight="15885" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
     <sheet name="Information" sheetId="2" r:id="rId2"/>
     <sheet name="L1_ChooseAStarter" sheetId="3" r:id="rId3"/>
+    <sheet name="B1_RivalBattleOffer" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>XLOOKUP</t>
   </si>
@@ -62,6 +63,18 @@
   </si>
   <si>
     <t xml:space="preserve">Time Remaining </t>
+  </si>
+  <si>
+    <t>Do you accept?</t>
+  </si>
+  <si>
+    <t>Your rival, [] offers you to battle, contesting for the [] function.</t>
+  </si>
+  <si>
+    <t>Unlocked functions:</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
@@ -469,7 +482,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -484,10 +497,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FEC854-5F2C-4439-9B10-91385C4E6F6F}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:D3"/>
+  <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -513,14 +526,23 @@
       <c r="B3" s="1"/>
       <c r="C3" s="2">
         <f ca="1">D3-NOW()</f>
-        <v>9.0181597217451781E-2</v>
+        <v>6.8509953700413462E-2</v>
       </c>
       <c r="D3" s="2">
         <v>45809.662609606479</v>
       </c>
     </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rj0B5JYqci1h/lqRC1ahyCTMcZHzmNQg98Pej68Ur7uJQe0diBpa8fqaK2MSFLaC7DPMzieNdJoZUM0Fqg0aqQ==" saltValue="R7DkZ+5Vy9VG8zZTowy73w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -533,7 +555,7 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -561,7 +583,32 @@
       <c r="C8" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IV8TLPBvCGQR47d9G6goayeZFTssMGfqzsIyX8zTfRwz1J+yJ7UgvO7C74FtCUKOH9KwUQzqYQ/Ik1OxyhN8mw==" saltValue="+YR3yY6BtJL6ni7ZkNRWVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataConsolidate/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578B9A5C-5C85-40AA-80A4-FD305EEEB547}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="B2:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Upload wb changes also.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF76ED51-DE43-4F57-BDA7-986F8CD6A577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BC8895-9FE2-4319-BD58-81334709370E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15885" activeTab="2" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
@@ -686,7 +686,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
@@ -711,7 +711,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="2">
         <f ca="1">D3-NOW()</f>
-        <v>-0.11988449074124219</v>
+        <v>-0.1245991898176726</v>
       </c>
       <c r="D3" s="2">
         <v>45809.662609606479</v>
@@ -742,8 +742,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>

</xml_diff>

<commit_message>
Remove unused files now that Unity is hooked up.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -1,24 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BC8895-9FE2-4319-BD58-81334709370E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70FA45F-8847-48C7-83C0-B3BCBF28974D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="38700" windowHeight="15885" activeTab="2" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15885" activeTab="3" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
     <sheet name="Information" sheetId="2" r:id="rId2"/>
-    <sheet name="L1_ChooseAStarter" sheetId="3" r:id="rId3"/>
-    <sheet name="B1_RivalBattleOffer" sheetId="4" r:id="rId4"/>
-    <sheet name="L2_Battle" sheetId="5" r:id="rId5"/>
-    <sheet name="L2_ExcelHQ" sheetId="6" r:id="rId6"/>
+    <sheet name="L2_Battle" sheetId="5" r:id="rId3"/>
+    <sheet name="UnityIsActive" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,19 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>XLOOKUP</t>
-  </si>
-  <si>
-    <t>INDEX</t>
-  </si>
-  <si>
-    <t>VLOOKUP</t>
-  </si>
-  <si>
-    <t>Selection:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Level Deadline</t>
   </si>
@@ -64,51 +50,12 @@
     <t xml:space="preserve">Time Remaining </t>
   </si>
   <si>
-    <t>Your rival, [] offers you to battle, contesting for the [] function.</t>
-  </si>
-  <si>
     <t>Unlocked functions:</t>
   </si>
   <si>
     <t>None</t>
   </si>
   <si>
-    <t>Please select your starting function, enter its name in the 'finished' box, and then recalculate the sheet.</t>
-  </si>
-  <si>
-    <t>Do you accept? (TRUE or FALSE)</t>
-  </si>
-  <si>
-    <t>You come to the Excel HQ with your unlocked functions.</t>
-  </si>
-  <si>
-    <t>Elliott Patterson</t>
-  </si>
-  <si>
-    <t>Option 1</t>
-  </si>
-  <si>
-    <t>Option 2</t>
-  </si>
-  <si>
-    <t>Option 3</t>
-  </si>
-  <si>
-    <t>Ha Dang</t>
-  </si>
-  <si>
-    <t>Julien Lacaze</t>
-  </si>
-  <si>
-    <t>…who deals in lookup functions</t>
-  </si>
-  <si>
-    <t>…who deals in manipulation functions</t>
-  </si>
-  <si>
-    <t>…who deals in aggregation functions</t>
-  </si>
-  <si>
     <t>Answer:</t>
   </si>
   <si>
@@ -136,7 +83,22 @@
     <t>https://projecteuler.net/</t>
   </si>
   <si>
-    <t>There are 3 purveyours in front of you… type in the number of the person you wish to fight.</t>
+    <t>Controls:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move: </t>
+  </si>
+  <si>
+    <t>Arrow keys</t>
+  </si>
+  <si>
+    <t>Spacebar:</t>
+  </si>
+  <si>
+    <t>Interact</t>
+  </si>
+  <si>
+    <t>Excel input is blocked - access through the overworld!</t>
   </si>
 </sst>
 </file>
@@ -146,16 +108,10 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,9 +245,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,10 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -671,7 +624,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <sheetData/>
@@ -686,7 +641,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
@@ -698,20 +655,20 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1"/>
       <c r="C3" s="2">
         <f ca="1">D3-NOW()</f>
-        <v>-0.1245991898176726</v>
+        <v>-3.1487115740746958</v>
       </c>
       <c r="D3" s="2">
         <v>45809.662609606479</v>
@@ -719,15 +676,15 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -738,77 +695,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEC1F9E8-8D01-42FA-A050-785391142542}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:F8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578B9A5C-5C85-40AA-80A4-FD305EEEB547}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="B2:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B6" s="4"/>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE00E63-6CB6-4E99-ACB4-864CD6BC5ACA}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:O22"/>
@@ -821,193 +707,193 @@
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O3" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>29</v>
+        <v>6</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O5" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="8"/>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="11"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="11"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="11"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="11"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="11"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="11"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="11"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="11"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="11"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="11"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="11"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B21" s="9"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="11"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B22" s="12"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="14"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="13"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -1022,67 +908,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289F557-B91D-41C4-BD26-03F6ABDAD362}">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="B2:F10"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5015013-787F-47F7-ACA7-7A0BFFA3385A}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="B2:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="25.92578125" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
-      <c r="B10" s="3"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Add the control instruction for opening and closing the menu.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29001"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70FA45F-8847-48C7-83C0-B3BCBF28974D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C44455C-1254-41B6-ADDE-66726C7240D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="38700" windowHeight="15885" activeTab="3" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15885" activeTab="3" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Level Deadline</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>Excel input is blocked - access through the overworld!</t>
+  </si>
+  <si>
+    <t>M:</t>
+  </si>
+  <si>
+    <t>Menu</t>
   </si>
 </sst>
 </file>
@@ -668,7 +674,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="2">
         <f ca="1">D3-NOW()</f>
-        <v>-3.1487115740746958</v>
+        <v>-5.3683346064863144</v>
       </c>
       <c r="D3" s="2">
         <v>45809.662609606479</v>
@@ -911,9 +917,11 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5015013-787F-47F7-ACA7-7A0BFFA3385A}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -943,6 +951,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Further adjustments to instructions.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C44455C-1254-41B6-ADDE-66726C7240D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B93D1F-70F3-4FA7-98EF-431422FDD137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="38700" windowHeight="15885" activeTab="3" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="38700" windowHeight="15885" activeTab="3" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Level Deadline</t>
   </si>
@@ -92,19 +92,22 @@
     <t>Arrow keys</t>
   </si>
   <si>
-    <t>Spacebar:</t>
-  </si>
-  <si>
-    <t>Interact</t>
-  </si>
-  <si>
-    <t>Excel input is blocked - access through the overworld!</t>
-  </si>
-  <si>
-    <t>M:</t>
-  </si>
-  <si>
-    <t>Menu</t>
+    <t>Excel input is currently blocked - access challenges through the overworld!</t>
+  </si>
+  <si>
+    <t>Select dialogue:</t>
+  </si>
+  <si>
+    <t>Interact:</t>
+  </si>
+  <si>
+    <t>Space/Return</t>
+  </si>
+  <si>
+    <t>Menu:</t>
+  </si>
+  <si>
+    <t>M</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -674,7 +677,7 @@
       <c r="B3" s="1"/>
       <c r="C3" s="2">
         <f ca="1">D3-NOW()</f>
-        <v>-5.3683346064863144</v>
+        <v>-5.3699662037033704</v>
       </c>
       <c r="D3" s="2">
         <v>45809.662609606479</v>
@@ -917,17 +920,18 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5015013-787F-47F7-ACA7-7A0BFFA3385A}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B2:C8"/>
+  <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.4">
@@ -945,18 +949,26 @@
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B9" t="s">
         <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start work on switching to the new battle system.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99B93D1F-70F3-4FA7-98EF-431422FDD137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59FF275-9DAB-4648-A2E1-2A7C36240993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="38700" windowHeight="15885" activeTab="3" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
-    <sheet name="Information" sheetId="2" r:id="rId2"/>
-    <sheet name="L2_Battle" sheetId="5" r:id="rId3"/>
-    <sheet name="UnityIsActive" sheetId="7" r:id="rId4"/>
+    <sheet name="Battle" sheetId="5" r:id="rId2"/>
+    <sheet name="UnityIsActive" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,22 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
-  <si>
-    <t>Level Deadline</t>
-  </si>
-  <si>
-    <t>Active Level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time Remaining </t>
-  </si>
-  <si>
-    <t>Unlocked functions:</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Answer:</t>
   </si>
@@ -69,9 +53,6 @@
   </si>
   <si>
     <t>[Question]</t>
-  </si>
-  <si>
-    <t>Locked functions:</t>
   </si>
   <si>
     <t>Credit for Questions to Project Euler</t>
@@ -114,9 +95,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="20"/>
@@ -148,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -160,21 +138,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -256,18 +219,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -277,12 +237,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -290,9 +250,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -646,263 +603,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3FEC854-5F2C-4439-9B10-91385C4E6F6F}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="2" max="2" width="20.78515625" customWidth="1"/>
-    <col min="3" max="3" width="21.0703125" customWidth="1"/>
-    <col min="4" max="4" width="23.640625" customWidth="1"/>
-    <col min="5" max="5" width="16.0703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2">
-        <f ca="1">D3-NOW()</f>
-        <v>-5.3699662037033704</v>
-      </c>
-      <c r="D3" s="2">
-        <v>45809.662609606479</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE00E63-6CB6-4E99-ACB4-864CD6BC5ACA}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B2:O22"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7"/>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="10"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="10"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="10"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="10"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="10"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="10"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B22" s="11"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="13"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="11"/>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -917,12 +816,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5015013-787F-47F7-ACA7-7A0BFFA3385A}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B2:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
@@ -931,44 +830,44 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write out case data.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59FF275-9DAB-4648-A2E1-2A7C36240993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5799DAAC-8E85-405B-BAAE-776BA43709FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
@@ -38,32 +38,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Answer:</t>
   </si>
   <si>
-    <t>[Player] challenges you to a battle for the [] function!</t>
-  </si>
-  <si>
-    <t>Here is the question, you have [] minutes (which you can follow on the 'Information' tab), go!</t>
-  </si>
-  <si>
-    <t>Note yada yada.</t>
-  </si>
-  <si>
     <t>[Question]</t>
   </si>
   <si>
-    <t>Credit for Questions to Project Euler</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
-  </si>
-  <si>
-    <t>https://projecteuler.net/</t>
-  </si>
-  <si>
     <t>Controls:</t>
   </si>
   <si>
@@ -89,6 +71,42 @@
   </si>
   <si>
     <t>M</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>PLAYER has challenged you to a battle!</t>
+  </si>
+  <si>
+    <t>Example answer format:</t>
+  </si>
+  <si>
+    <t>Question credit:</t>
+  </si>
+  <si>
+    <t>Question:</t>
+  </si>
+  <si>
+    <t>DATA [1]</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Question Id:</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Please solve this question on the WORKINGS tab.  Note that you will not be able to use functions you have not yet unlocked there.</t>
+  </si>
+  <si>
+    <t>Here is the question, you have [] minutes (which you can follow in the overworld window).</t>
+  </si>
+  <si>
+    <t>(Some text may not be directly visible on some long questions.)</t>
   </si>
 </sst>
 </file>
@@ -104,9 +122,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="20"/>
-      <color theme="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -215,16 +232,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -237,9 +252,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -252,9 +264,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,10 +623,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE00E63-6CB6-4E99-ACB4-864CD6BC5ACA}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B2:O22"/>
+  <dimension ref="B2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -617,183 +635,139 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>6</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O5" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="O6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="8"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="8"/>
+      <c r="B10" s="12" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="8"/>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B13" s="6"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="8"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="8"/>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="8"/>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="8"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="10"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="10"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="8"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="8"/>
+      <c r="B20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="8"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B22" s="9"/>
+      <c r="B22" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -801,18 +775,84 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="11"/>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="B9:J22"/>
+    <mergeCell ref="B15:I18"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="O4" r:id="rId1" xr:uid="{38BF5EE4-1F6F-4480-86C3-EB83AEF27EF9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -830,44 +870,44 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.4">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lock example answer cell, remove unused code.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5799DAAC-8E85-405B-BAAE-776BA43709FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E2534C-13C4-4BF4-9330-5E2C52BB3A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
@@ -235,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -271,6 +271,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -626,7 +627,7 @@
   <dimension ref="B2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -649,7 +650,7 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="13"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O5" t="s">

</xml_diff>

<commit_message>
Add instruction to write -1 if you give up on a challenge.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E2534C-13C4-4BF4-9330-5E2C52BB3A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F848413A-8143-491A-90EA-AECBC3CBA827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Answer:</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>(Some text may not be directly visible on some long questions.)</t>
+  </si>
+  <si>
+    <t>If you give up, write '-1' as the answer.</t>
   </si>
 </sst>
 </file>
@@ -624,11 +627,9 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFE00E63-6CB6-4E99-ACB4-864CD6BC5ACA}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="B2:O29"/>
+  <dimension ref="B2:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -677,81 +678,62 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B13" t="s">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.4">
+      <c r="B15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B15" s="2" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B16" s="5"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B17" s="5"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="10"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="9"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="6"/>
       <c r="J18" s="10"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="6"/>
       <c r="J19" s="10"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
       <c r="J20" s="10"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.4">
@@ -767,7 +749,7 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B22" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -790,7 +772,9 @@
       <c r="J23" s="10"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B24" s="10"/>
+      <c r="B24" s="10" t="s">
+        <v>17</v>
+      </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -812,6 +796,14 @@
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
       <c r="J26" s="10"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.4">
@@ -826,14 +818,6 @@
       <c r="J27" s="10"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B28" s="10"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
       <c r="J28" s="10"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.4">
@@ -847,10 +831,32 @@
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
     </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="1">
-    <mergeCell ref="B15:I18"/>
+    <mergeCell ref="B17:I20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Euler problems up to #11.  Fix issue with writing in data.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F848413A-8143-491A-90EA-AECBC3CBA827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71526567-F875-48FF-9EE2-F2826CB36F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
@@ -243,38 +243,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,7 +651,7 @@
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.4">
       <c r="O5" t="s">
@@ -672,7 +672,7 @@
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.4">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -692,166 +692,166 @@
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="4"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B18" s="5"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="10"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B19" s="5"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="10"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="2"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="10"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="J28" s="10"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B30" s="10"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.4">
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
     </row>
   </sheetData>
   <dataConsolidate/>

</xml_diff>

<commit_message>
Fix issues discovered by Dim.
</commit_message>
<xml_diff>
--- a/ExcelDynamicCase/ExcelDynamicCase.xlsx
+++ b/ExcelDynamicCase/ExcelDynamicCase.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29005"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harry\source\repos\ExcelDynamicCase\ExcelDynamicCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71526567-F875-48FF-9EE2-F2826CB36F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FCC652-191B-436A-AAB5-CF51C563C7AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="38700" windowHeight="15885" activeTab="1" xr2:uid="{A4107E39-ADFC-428B-BEC0-F1C599043212}"/>
   </bookViews>
   <sheets>
     <sheet name="Workings" sheetId="1" r:id="rId1"/>
@@ -691,7 +691,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:10" ht="57" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B17" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>